<commit_message>
done 28th string problem
</commit_message>
<xml_diff>
--- a/dsa questions babbar.xlsx
+++ b/dsa questions babbar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA\babbar sheet sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E40683-FFB4-4360-AB08-CE876B896E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4794B9B3-1790-4E48-8D80-CC8396CCBE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1936,15 +1936,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1968,6 +1959,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2256,8 +2256,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:XFC485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="22.2" zeroHeight="1" x14ac:dyDescent="0.45"/>
@@ -2296,8 +2296,8 @@
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" s="63" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:4" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="74" t="s">
         <v>485</v>
       </c>
     </row>
@@ -2742,8 +2742,8 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:4" s="64" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="64" t="s">
+    <row r="44" spans="1:4" s="75" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="75" t="s">
         <v>489</v>
       </c>
     </row>
@@ -2872,8 +2872,8 @@
       <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="1:4" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="65" t="s">
+    <row r="57" spans="1:4" s="76" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="76" t="s">
         <v>490</v>
       </c>
     </row>
@@ -3198,16 +3198,17 @@
       </c>
       <c r="D84" s="20"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A85" s="9">
+    <row r="85" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="13">
         <v>28</v>
       </c>
-      <c r="B85" s="27" t="s">
+      <c r="B85" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="14" t="s">
         <v>78</v>
       </c>
+      <c r="D85" s="17"/>
     </row>
     <row r="86" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A86" s="13">
@@ -7860,8 +7861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F90590-BFBE-4C68-82AE-A25E3E5CE8C8}">
   <dimension ref="A1:AA1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="22.2" zeroHeight="1" x14ac:dyDescent="0.45"/>
@@ -7875,25 +7876,25 @@
   <sheetData>
     <row r="1" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="39"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="68" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="69" t="s">
         <v>461</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="70" t="s">
         <v>460</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="71" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="75"/>
-      <c r="B3" s="76" t="s">
+      <c r="A3" s="72"/>
+      <c r="B3" s="73" t="s">
         <v>463</v>
       </c>
       <c r="C3" s="41"/>
@@ -8460,7 +8461,7 @@
     <row r="53" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="35"/>
     </row>
-    <row r="54" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="39">
         <v>1</v>
       </c>
@@ -8471,7 +8472,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="39">
         <v>2</v>
       </c>
@@ -8482,7 +8483,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="39">
         <v>3</v>
       </c>
@@ -8493,7 +8494,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="39">
         <v>4</v>
       </c>
@@ -8504,7 +8505,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="39">
         <v>5</v>
       </c>
@@ -8515,7 +8516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="39">
         <v>6</v>
       </c>
@@ -8526,7 +8527,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="39">
         <v>7</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="39">
         <v>8</v>
       </c>
@@ -8548,7 +8549,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="39">
         <v>9</v>
       </c>
@@ -8559,7 +8560,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="39">
         <v>10</v>
       </c>
@@ -8570,7 +8571,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="39">
         <v>11</v>
       </c>
@@ -8581,7 +8582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="39">
         <v>12</v>
       </c>
@@ -8592,7 +8593,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="39">
         <v>13</v>
       </c>
@@ -8603,7 +8604,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="39">
         <v>14</v>
       </c>
@@ -8614,7 +8615,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="39">
         <v>15</v>
       </c>
@@ -8625,7 +8626,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="39">
         <v>16</v>
       </c>
@@ -8636,7 +8637,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="39">
         <v>17</v>
       </c>
@@ -8647,7 +8648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="39">
         <v>18</v>
       </c>
@@ -8658,7 +8659,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="39">
         <v>19</v>
       </c>
@@ -8669,7 +8670,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="39">
         <v>20</v>
       </c>
@@ -8680,7 +8681,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="66" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" s="63" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="39">
         <v>21</v>
       </c>
@@ -8794,10 +8795,10 @@
       <c r="A84" s="13">
         <v>32</v>
       </c>
-      <c r="B84" s="67" t="s">
+      <c r="B84" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="65" t="s">
         <v>81</v>
       </c>
     </row>
@@ -8805,10 +8806,10 @@
       <c r="A85" s="13">
         <v>33</v>
       </c>
-      <c r="B85" s="67" t="s">
+      <c r="B85" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="65" t="s">
         <v>82</v>
       </c>
     </row>
@@ -8816,10 +8817,10 @@
       <c r="A86" s="13">
         <v>34</v>
       </c>
-      <c r="B86" s="67" t="s">
+      <c r="B86" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="65" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8827,10 +8828,10 @@
       <c r="A87" s="13">
         <v>35</v>
       </c>
-      <c r="B87" s="67" t="s">
+      <c r="B87" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="65" t="s">
         <v>84</v>
       </c>
     </row>
@@ -8838,10 +8839,10 @@
       <c r="A88" s="13">
         <v>36</v>
       </c>
-      <c r="B88" s="67" t="s">
+      <c r="B88" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C88" s="68" t="s">
+      <c r="C88" s="65" t="s">
         <v>85</v>
       </c>
     </row>
@@ -8849,10 +8850,10 @@
       <c r="A89" s="13">
         <v>37</v>
       </c>
-      <c r="B89" s="67" t="s">
+      <c r="B89" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="68" t="s">
+      <c r="C89" s="65" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8860,10 +8861,10 @@
       <c r="A90" s="13">
         <v>38</v>
       </c>
-      <c r="B90" s="67" t="s">
+      <c r="B90" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C90" s="65" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8871,10 +8872,10 @@
       <c r="A91" s="13">
         <v>39</v>
       </c>
-      <c r="B91" s="67" t="s">
+      <c r="B91" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="68" t="s">
+      <c r="C91" s="65" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8882,10 +8883,10 @@
       <c r="A92" s="13">
         <v>40</v>
       </c>
-      <c r="B92" s="67" t="s">
+      <c r="B92" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C92" s="68" t="s">
+      <c r="C92" s="65" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8893,10 +8894,10 @@
       <c r="A93" s="13">
         <v>41</v>
       </c>
-      <c r="B93" s="67" t="s">
+      <c r="B93" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="68" t="s">
+      <c r="C93" s="65" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8904,17 +8905,17 @@
       <c r="A94" s="13">
         <v>42</v>
       </c>
-      <c r="B94" s="67" t="s">
+      <c r="B94" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C94" s="68" t="s">
+      <c r="C94" s="65" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="16" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="13"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="68"/>
+      <c r="B95" s="66"/>
+      <c r="C95" s="65"/>
     </row>
     <row r="96" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="97" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
done 32 rearrange string
</commit_message>
<xml_diff>
--- a/dsa questions babbar.xlsx
+++ b/dsa questions babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA\babbar sheet sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC4959F-5561-4C0F-9BCF-93C297B4411B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAC7E2A-BE8F-4D06-9CF9-DA072817FC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="885" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2257,8 +2257,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:XFC485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="22.2" zeroHeight="1" x14ac:dyDescent="0.45"/>
@@ -3249,16 +3249,17 @@
       </c>
       <c r="D88" s="17"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A89" s="9">
+    <row r="89" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="13">
         <v>32</v>
       </c>
-      <c r="B89" s="27" t="s">
+      <c r="B89" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="14" t="s">
         <v>82</v>
       </c>
+      <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="9">
@@ -7871,7 +7872,7 @@
   <dimension ref="A1:AA1011"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="22.2" zeroHeight="1" x14ac:dyDescent="0.45"/>
@@ -8800,25 +8801,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="16" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="13">
+    <row r="84" spans="1:3" s="42" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="39">
         <v>32</v>
       </c>
-      <c r="B84" s="64" t="s">
+      <c r="B84" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C84" s="65" t="s">
+      <c r="C84" s="41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="16" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="13">
+    <row r="85" spans="1:3" s="42" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="39">
         <v>33</v>
       </c>
-      <c r="B85" s="64" t="s">
+      <c r="B85" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C85" s="65" t="s">
+      <c r="C85" s="41" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>